<commit_message>
Make sure that we have 70% of bugs in train and 30% in test
</commit_message>
<xml_diff>
--- a/output/2_0_0/nomogram_config_2_0_0.xlsx
+++ b/output/2_0_0/nomogram_config_2_0_0.xlsx
@@ -466,7 +466,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>-0.2235</v>
+        <v>-1.1158</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -482,7 +482,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>-0.0145</v>
+        <v>-0.0233</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -499,7 +499,7 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.09909999999999999</v>
+        <v>0.1614</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -516,7 +516,7 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>-0.1142</v>
+        <v>-0.0606</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -533,7 +533,7 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>-0.1383</v>
+        <v>0.066</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -550,7 +550,7 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>-0.2581</v>
+        <v>-0.8298</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -567,7 +567,7 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.014</v>
+        <v>0.0209</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -584,7 +584,7 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>-0.007</v>
+        <v>0.0402</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -601,7 +601,7 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.0001</v>
+        <v>0.0013</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -618,7 +618,7 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.039</v>
+        <v>0.0086</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -635,7 +635,7 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>-0.2469</v>
+        <v>0.06950000000000001</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -652,7 +652,7 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>-0.0095</v>
+        <v>0.0008</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -669,7 +669,7 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>-0.3129</v>
+        <v>-1.2648</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -686,7 +686,7 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>-0.0535</v>
+        <v>-0.073</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -703,7 +703,7 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>-0.0002</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -720,7 +720,7 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>-0.0762</v>
+        <v>-0.0029</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -737,7 +737,7 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>0.0172</v>
+        <v>0.0186</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -754,7 +754,7 @@
         <v>25</v>
       </c>
       <c r="B20">
-        <v>0.1198</v>
+        <v>0.542</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -771,7 +771,7 @@
         <v>26</v>
       </c>
       <c r="B21">
-        <v>0.0313</v>
+        <v>0.031</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -788,7 +788,7 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0.0066</v>
+        <v>-0.0005</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -805,7 +805,7 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.0183</v>
+        <v>0.1513</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -822,7 +822,7 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>-0.0571</v>
+        <v>0.1722</v>
       </c>
       <c r="C24">
         <v>0</v>

</xml_diff>